<commit_message>
Atualiza BASE.xlsx automático (Google Sheets)
</commit_message>
<xml_diff>
--- a/public/data/BASE.xlsx
+++ b/public/data/BASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gondaski.sharepoint.com/sites/OperaesePeas/Documentos Compartilhados/Operações/Suprimentos/Logística/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1420" documentId="13_ncr:1_{1FFCA2AD-14E4-4B9A-98FB-D1DA18665813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7706D0D-5EF7-477A-B129-C1A767F7B328}"/>
+  <xr:revisionPtr revIDLastSave="1426" documentId="13_ncr:1_{1FFCA2AD-14E4-4B9A-98FB-D1DA18665813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F16A2B63-BB11-40F5-96D4-AE4A77C2ACD0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="1" xr2:uid="{79B5BA07-D2C6-4A71-9E5E-B065B1438F00}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{79B5BA07-D2C6-4A71-9E5E-B065B1438F00}"/>
   </bookViews>
   <sheets>
     <sheet name="VW DAF" sheetId="9" r:id="rId1"/>
@@ -4559,7 +4559,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5009,6 +5009,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5038,54 +5041,6 @@
     </xf>
     <xf numFmtId="0" fontId="43" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7405,39 +7360,39 @@
       <c r="C27" s="39"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="164" t="s">
+      <c r="A28" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="167"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="164" t="s">
+      <c r="A29" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="165"/>
-      <c r="C29" s="166"/>
+      <c r="B29" s="166"/>
+      <c r="C29" s="167"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="164" t="s">
+      <c r="A30" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="165"/>
-      <c r="C30" s="166"/>
+      <c r="B30" s="166"/>
+      <c r="C30" s="167"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="164" t="s">
+      <c r="A31" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="165"/>
-      <c r="C31" s="166"/>
+      <c r="B31" s="166"/>
+      <c r="C31" s="167"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="164" t="s">
+      <c r="A32" s="165" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="165"/>
-      <c r="C32" s="166"/>
+      <c r="B32" s="166"/>
+      <c r="C32" s="167"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="29"/>
@@ -7514,18 +7469,18 @@
       <c r="C40" s="30"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="161" t="s">
+      <c r="A41" s="162" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="162"/>
-      <c r="C41" s="163"/>
+      <c r="B41" s="163"/>
+      <c r="C41" s="164"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="161" t="s">
+      <c r="A42" s="162" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="162"/>
-      <c r="C42" s="163"/>
+      <c r="B42" s="163"/>
+      <c r="C42" s="164"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="30"/>
@@ -7699,8 +7654,8 @@
   <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.45"/>
@@ -12659,58 +12614,58 @@
       </c>
     </row>
     <row r="52" spans="1:20" ht="15">
-      <c r="A52" s="179" t="s">
+      <c r="A52" s="14" t="s">
         <v>276</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C52" s="181">
+      <c r="C52" s="154">
         <f>IFERROR((D52*1.5)/1440, "?")</f>
         <v>0.49791666666666667</v>
       </c>
-      <c r="D52" s="180">
+      <c r="D52" s="12">
         <v>478</v>
       </c>
-      <c r="E52" s="182">
+      <c r="E52" s="155">
         <f>IFERROR((D52*6),"?")</f>
         <v>2868</v>
       </c>
-      <c r="F52" s="183"/>
-      <c r="G52" s="180" t="s">
+      <c r="F52" s="156"/>
+      <c r="G52" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="H52" s="184">
+      <c r="H52" s="157">
         <v>45978</v>
       </c>
-      <c r="I52" s="185" t="s">
+      <c r="I52" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="J52" s="180" t="s">
+      <c r="J52" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="K52" s="180" t="s">
+      <c r="K52" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="L52" s="180" t="s">
+      <c r="L52" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="M52" s="180" t="s">
+      <c r="M52" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N52" s="179" t="s">
+      <c r="N52" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="O52" s="180" t="s">
+      <c r="O52" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="P52" s="186" t="s">
+      <c r="P52" s="161" t="s">
         <v>248</v>
       </c>
-      <c r="Q52" s="180" t="s">
+      <c r="Q52" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="R52" s="180" t="s">
+      <c r="R52" s="12" t="s">
         <v>101</v>
       </c>
       <c r="S52" s="2" t="str">
@@ -12763,58 +12718,58 @@
       </c>
     </row>
     <row r="53" spans="1:20" ht="15">
-      <c r="A53" s="179" t="s">
+      <c r="A53" s="14" t="s">
         <v>276</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C53" s="181">
+      <c r="C53" s="154">
         <f>IFERROR((D53*1.5)/1440, "?")</f>
         <v>0.49791666666666667</v>
       </c>
-      <c r="D53" s="180">
+      <c r="D53" s="12">
         <v>478</v>
       </c>
-      <c r="E53" s="182">
+      <c r="E53" s="155">
         <f>IFERROR((D53*6),"?")</f>
         <v>2868</v>
       </c>
-      <c r="F53" s="183"/>
-      <c r="G53" s="180" t="s">
+      <c r="F53" s="156"/>
+      <c r="G53" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="H53" s="184">
+      <c r="H53" s="157">
         <v>45978</v>
       </c>
-      <c r="I53" s="185" t="s">
+      <c r="I53" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="J53" s="180" t="s">
+      <c r="J53" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="K53" s="180" t="s">
+      <c r="K53" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="L53" s="180" t="s">
+      <c r="L53" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="M53" s="180" t="s">
+      <c r="M53" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N53" s="179" t="s">
+      <c r="N53" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="O53" s="180" t="s">
+      <c r="O53" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="P53" s="186" t="s">
+      <c r="P53" s="161" t="s">
         <v>248</v>
       </c>
-      <c r="Q53" s="180" t="s">
+      <c r="Q53" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="R53" s="180" t="s">
+      <c r="R53" s="12" t="s">
         <v>101</v>
       </c>
       <c r="S53" s="2" t="str">
@@ -12867,58 +12822,58 @@
       </c>
     </row>
     <row r="54" spans="1:20" ht="15">
-      <c r="A54" s="179" t="s">
+      <c r="A54" s="14" t="s">
         <v>276</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C54" s="181">
+      <c r="C54" s="154">
         <f>IFERROR((D54*1.5)/1440, "?")</f>
         <v>0.31874999999999998</v>
       </c>
-      <c r="D54" s="180">
+      <c r="D54" s="12">
         <v>306</v>
       </c>
-      <c r="E54" s="182">
+      <c r="E54" s="155">
         <f>IFERROR((D54*6),"?")</f>
         <v>1836</v>
       </c>
-      <c r="F54" s="183"/>
-      <c r="G54" s="180" t="s">
+      <c r="F54" s="156"/>
+      <c r="G54" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="H54" s="184">
+      <c r="H54" s="157">
         <v>45978</v>
       </c>
-      <c r="I54" s="185" t="s">
+      <c r="I54" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="J54" s="180" t="s">
+      <c r="J54" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="K54" s="180" t="s">
+      <c r="K54" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="L54" s="180" t="s">
+      <c r="L54" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="M54" s="180" t="s">
+      <c r="M54" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N54" s="179" t="s">
+      <c r="N54" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="O54" s="180" t="s">
+      <c r="O54" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="P54" s="186" t="s">
+      <c r="P54" s="161" t="s">
         <v>248</v>
       </c>
-      <c r="Q54" s="180" t="s">
+      <c r="Q54" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="R54" s="180" t="s">
+      <c r="R54" s="12" t="s">
         <v>148</v>
       </c>
       <c r="S54" s="2" t="str">
@@ -12964,58 +12919,58 @@
       </c>
     </row>
     <row r="55" spans="1:20" ht="15">
-      <c r="A55" s="179" t="s">
+      <c r="A55" s="14" t="s">
         <v>276</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C55" s="181">
+      <c r="C55" s="154">
         <f>IFERROR((D55*1.5)/1440, "?")</f>
         <v>0.31874999999999998</v>
       </c>
-      <c r="D55" s="180">
+      <c r="D55" s="12">
         <v>306</v>
       </c>
-      <c r="E55" s="182">
+      <c r="E55" s="155">
         <f>IFERROR((D55*6),"?")</f>
         <v>1836</v>
       </c>
-      <c r="F55" s="183"/>
-      <c r="G55" s="180" t="s">
+      <c r="F55" s="156"/>
+      <c r="G55" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="H55" s="184">
+      <c r="H55" s="157">
         <v>45978</v>
       </c>
-      <c r="I55" s="185" t="s">
+      <c r="I55" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="J55" s="180" t="s">
+      <c r="J55" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="K55" s="180" t="s">
+      <c r="K55" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="L55" s="180" t="s">
+      <c r="L55" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="M55" s="180" t="s">
+      <c r="M55" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N55" s="179" t="s">
+      <c r="N55" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="O55" s="180" t="s">
+      <c r="O55" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="P55" s="186" t="s">
+      <c r="P55" s="161" t="s">
         <v>248</v>
       </c>
-      <c r="Q55" s="180" t="s">
+      <c r="Q55" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="R55" s="180" t="s">
+      <c r="R55" s="12" t="s">
         <v>148</v>
       </c>
       <c r="S55" s="2" t="str">
@@ -18130,7 +18085,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="15" customHeight="1">
-      <c r="A69" s="171" t="s">
+      <c r="A69" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -18139,23 +18094,23 @@
       <c r="C69" s="18">
         <v>45971</v>
       </c>
-      <c r="D69" s="174" t="s">
+      <c r="D69" s="82" t="s">
         <v>465</v>
       </c>
-      <c r="E69" s="172" t="str">
+      <c r="E69" s="1" t="str">
         <f>_xlfn.XLOOKUP(F69,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>056953013</v>
       </c>
       <c r="F69" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="G69" s="176">
+      <c r="G69" s="16">
         <v>884.29</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="I69" s="175">
+      <c r="I69" s="17">
         <v>778</v>
       </c>
       <c r="J69" s="18">
@@ -18164,13 +18119,13 @@
       <c r="K69" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="L69" s="178" t="str">
+      <c r="L69" s="17" t="str">
         <f>TEXT($C69,"dd.mm") &amp; " -Ped " &amp; D69 &amp; " -" &amp; F69 &amp; " -R$" &amp; G69 &amp; IF(LEN(TRIM(I69))=0, "", " -NF " &amp; TRIM(I69))</f>
         <v>10.11 -Ped 047757 -CARGADEDICADA TRANS -R$884,29 -NF 778</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="15" customHeight="1">
-      <c r="A70" s="171" t="s">
+      <c r="A70" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -18179,23 +18134,23 @@
       <c r="C70" s="18">
         <v>45971</v>
       </c>
-      <c r="D70" s="174" t="s">
+      <c r="D70" s="82" t="s">
         <v>465</v>
       </c>
-      <c r="E70" s="172" t="str">
+      <c r="E70" s="1" t="str">
         <f>_xlfn.XLOOKUP(F70,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>056953013</v>
       </c>
       <c r="F70" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="G70" s="176">
+      <c r="G70" s="16">
         <v>884.29</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="I70" s="175">
+      <c r="I70" s="17">
         <v>779</v>
       </c>
       <c r="J70" s="18">
@@ -18204,13 +18159,13 @@
       <c r="K70" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="L70" s="178" t="str">
+      <c r="L70" s="17" t="str">
         <f>TEXT($C70,"dd.mm") &amp; " -Ped " &amp; D70 &amp; " -" &amp; F70 &amp; " -R$" &amp; G70 &amp; IF(LEN(TRIM(I70))=0, "", " -NF " &amp; TRIM(I70))</f>
         <v>10.11 -Ped 047757 -CARGADEDICADA TRANS -R$884,29 -NF 779</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="15" customHeight="1">
-      <c r="A71" s="171" t="s">
+      <c r="A71" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -18219,23 +18174,23 @@
       <c r="C71" s="18">
         <v>45971</v>
       </c>
-      <c r="D71" s="174" t="s">
+      <c r="D71" s="82" t="s">
         <v>465</v>
       </c>
-      <c r="E71" s="172" t="str">
+      <c r="E71" s="1" t="str">
         <f>_xlfn.XLOOKUP(F71,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>056953013</v>
       </c>
       <c r="F71" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="G71" s="176">
+      <c r="G71" s="16">
         <v>884.29</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="I71" s="175">
+      <c r="I71" s="17">
         <v>781</v>
       </c>
       <c r="J71" s="18">
@@ -18244,13 +18199,13 @@
       <c r="K71" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="L71" s="178" t="str">
+      <c r="L71" s="17" t="str">
         <f>TEXT($C71,"dd.mm") &amp; " -Ped " &amp; D71 &amp; " -" &amp; F71 &amp; " -R$" &amp; G71 &amp; IF(LEN(TRIM(I71))=0, "", " -NF " &amp; TRIM(I71))</f>
         <v>10.11 -Ped 047757 -CARGADEDICADA TRANS -R$884,29 -NF 781</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="15" customHeight="1">
-      <c r="A72" s="171" t="s">
+      <c r="A72" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -18259,23 +18214,23 @@
       <c r="C72" s="18">
         <v>45971</v>
       </c>
-      <c r="D72" s="174" t="s">
+      <c r="D72" s="82" t="s">
         <v>465</v>
       </c>
-      <c r="E72" s="172" t="str">
+      <c r="E72" s="1" t="str">
         <f>_xlfn.XLOOKUP(F72,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>056953013</v>
       </c>
       <c r="F72" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="G72" s="176">
+      <c r="G72" s="16">
         <v>884.29</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="I72" s="175">
+      <c r="I72" s="17">
         <v>782</v>
       </c>
       <c r="J72" s="18">
@@ -18284,7 +18239,7 @@
       <c r="K72" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="L72" s="178" t="str">
+      <c r="L72" s="17" t="str">
         <f>TEXT($C72,"dd.mm") &amp; " -Ped " &amp; D72 &amp; " -" &amp; F72 &amp; " -R$" &amp; G72 &amp; IF(LEN(TRIM(I72))=0, "", " -NF " &amp; TRIM(I72))</f>
         <v>10.11 -Ped 047757 -CARGADEDICADA TRANS -R$884,29 -NF 782</v>
       </c>
@@ -18293,545 +18248,381 @@
       <c r="A73" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="B73" s="172" t="s">
+      <c r="B73" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C73" s="173">
+      <c r="C73" s="18">
         <v>45974</v>
       </c>
-      <c r="D73" s="174" t="s">
+      <c r="D73" s="82" t="s">
         <v>468</v>
       </c>
-      <c r="E73" s="172" t="str">
+      <c r="E73" s="1" t="str">
         <f>_xlfn.XLOOKUP(F73,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>061028125</v>
       </c>
       <c r="F73" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G73" s="176">
+      <c r="G73" s="16">
         <v>270</v>
       </c>
-      <c r="H73" s="171"/>
-      <c r="I73" s="175"/>
-      <c r="J73" s="173"/>
-      <c r="K73" s="177" t="s">
+      <c r="H73" s="4"/>
+      <c r="K73" s="81" t="s">
         <v>470</v>
       </c>
-      <c r="L73" s="178" t="str">
+      <c r="L73" s="17" t="str">
         <f t="shared" ref="L73:L76" si="2">TEXT($C73,"dd.mm") &amp; " -Ped " &amp; D73 &amp; " -" &amp; F73 &amp; " -R$" &amp; G73 &amp; IF(LEN(TRIM(I73))=0, "", " -NF " &amp; TRIM(I73))</f>
         <v>13.11 -Ped 047758 -INCOMESPMUNCK TRANSP -R$270</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="15" customHeight="1">
-      <c r="A74" s="171"/>
-      <c r="B74" s="172"/>
-      <c r="C74" s="173"/>
-      <c r="D74" s="174"/>
-      <c r="E74" s="172" t="str">
+      <c r="A74" s="4"/>
+      <c r="E74" s="1" t="str">
         <f>_xlfn.XLOOKUP(F74,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G74" s="176"/>
-      <c r="H74" s="171"/>
-      <c r="I74" s="175"/>
-      <c r="J74" s="173"/>
-      <c r="K74" s="177"/>
-      <c r="L74" s="178" t="str">
+      <c r="H74" s="4"/>
+      <c r="K74" s="81"/>
+      <c r="L74" s="17" t="str">
         <f t="shared" si="2"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="15" customHeight="1">
-      <c r="A75" s="171"/>
-      <c r="B75" s="172"/>
-      <c r="C75" s="173"/>
-      <c r="D75" s="174"/>
-      <c r="E75" s="172" t="str">
+      <c r="A75" s="4"/>
+      <c r="E75" s="1" t="str">
         <f>_xlfn.XLOOKUP(F75,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G75" s="176"/>
-      <c r="H75" s="171"/>
-      <c r="I75" s="175"/>
-      <c r="J75" s="173"/>
-      <c r="K75" s="177"/>
-      <c r="L75" s="178" t="str">
+      <c r="H75" s="4"/>
+      <c r="K75" s="81"/>
+      <c r="L75" s="17" t="str">
         <f t="shared" si="2"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="15" customHeight="1">
-      <c r="A76" s="171"/>
-      <c r="B76" s="172"/>
-      <c r="C76" s="173"/>
-      <c r="D76" s="174"/>
-      <c r="E76" s="172" t="str">
+      <c r="A76" s="4"/>
+      <c r="E76" s="1" t="str">
         <f>_xlfn.XLOOKUP(F76,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G76" s="176"/>
-      <c r="H76" s="171"/>
-      <c r="I76" s="175"/>
-      <c r="J76" s="173"/>
-      <c r="K76" s="177"/>
-      <c r="L76" s="178" t="str">
+      <c r="H76" s="4"/>
+      <c r="K76" s="81"/>
+      <c r="L76" s="17" t="str">
         <f t="shared" si="2"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="15" customHeight="1">
-      <c r="A77" s="171"/>
-      <c r="B77" s="172"/>
-      <c r="C77" s="173"/>
-      <c r="D77" s="174"/>
-      <c r="E77" s="172" t="str">
+      <c r="A77" s="4"/>
+      <c r="E77" s="1" t="str">
         <f>_xlfn.XLOOKUP(F77,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G77" s="176"/>
-      <c r="H77" s="171"/>
-      <c r="I77" s="175"/>
-      <c r="J77" s="173"/>
-      <c r="K77" s="177"/>
-      <c r="L77" s="178" t="str">
+      <c r="H77" s="4"/>
+      <c r="K77" s="81"/>
+      <c r="L77" s="17" t="str">
         <f t="shared" ref="L77:L99" si="3">TEXT($C77,"dd.mm") &amp; " -Ped " &amp; D77 &amp; " -" &amp; F77 &amp; " -R$" &amp; G77 &amp; IF(LEN(TRIM(I77))=0, "", " -NF " &amp; TRIM(I77))</f>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="15" customHeight="1">
-      <c r="A78" s="171"/>
-      <c r="B78" s="172"/>
-      <c r="C78" s="173"/>
-      <c r="D78" s="174"/>
-      <c r="E78" s="172" t="str">
+      <c r="A78" s="4"/>
+      <c r="E78" s="1" t="str">
         <f>_xlfn.XLOOKUP(F78,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G78" s="176"/>
-      <c r="H78" s="171"/>
-      <c r="I78" s="175"/>
-      <c r="J78" s="173"/>
-      <c r="K78" s="177"/>
-      <c r="L78" s="178" t="str">
+      <c r="H78" s="4"/>
+      <c r="K78" s="81"/>
+      <c r="L78" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="15" customHeight="1">
-      <c r="A79" s="171"/>
-      <c r="B79" s="172"/>
-      <c r="C79" s="173"/>
-      <c r="D79" s="174"/>
-      <c r="E79" s="172" t="str">
+      <c r="A79" s="4"/>
+      <c r="E79" s="1" t="str">
         <f>_xlfn.XLOOKUP(F79,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G79" s="176"/>
-      <c r="H79" s="171"/>
-      <c r="I79" s="175"/>
-      <c r="J79" s="173"/>
-      <c r="K79" s="177"/>
-      <c r="L79" s="178" t="str">
+      <c r="H79" s="4"/>
+      <c r="K79" s="81"/>
+      <c r="L79" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="15" customHeight="1">
-      <c r="A80" s="171"/>
-      <c r="B80" s="172"/>
-      <c r="C80" s="173"/>
-      <c r="D80" s="174"/>
-      <c r="E80" s="172" t="str">
+      <c r="A80" s="4"/>
+      <c r="E80" s="1" t="str">
         <f>_xlfn.XLOOKUP(F80,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G80" s="176"/>
-      <c r="H80" s="171"/>
-      <c r="I80" s="175"/>
-      <c r="J80" s="173"/>
-      <c r="K80" s="177"/>
-      <c r="L80" s="178" t="str">
+      <c r="H80" s="4"/>
+      <c r="K80" s="81"/>
+      <c r="L80" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="15" customHeight="1">
-      <c r="A81" s="171"/>
-      <c r="B81" s="172"/>
-      <c r="C81" s="173"/>
-      <c r="D81" s="174"/>
-      <c r="E81" s="172" t="str">
+      <c r="A81" s="4"/>
+      <c r="E81" s="1" t="str">
         <f>_xlfn.XLOOKUP(F81,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G81" s="176"/>
-      <c r="H81" s="171"/>
-      <c r="I81" s="175"/>
-      <c r="J81" s="173"/>
-      <c r="K81" s="177"/>
-      <c r="L81" s="178" t="str">
+      <c r="H81" s="4"/>
+      <c r="K81" s="81"/>
+      <c r="L81" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="15" customHeight="1">
-      <c r="A82" s="171"/>
-      <c r="B82" s="172"/>
-      <c r="C82" s="173"/>
-      <c r="D82" s="174"/>
-      <c r="E82" s="172" t="str">
+      <c r="A82" s="4"/>
+      <c r="E82" s="1" t="str">
         <f>_xlfn.XLOOKUP(F82,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G82" s="176"/>
-      <c r="H82" s="171"/>
-      <c r="I82" s="175"/>
-      <c r="J82" s="173"/>
-      <c r="K82" s="177"/>
-      <c r="L82" s="178" t="str">
+      <c r="H82" s="4"/>
+      <c r="K82" s="81"/>
+      <c r="L82" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="15" customHeight="1">
-      <c r="A83" s="171"/>
-      <c r="B83" s="172"/>
-      <c r="C83" s="173"/>
-      <c r="D83" s="174"/>
-      <c r="E83" s="172" t="str">
+      <c r="A83" s="4"/>
+      <c r="E83" s="1" t="str">
         <f>_xlfn.XLOOKUP(F83,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G83" s="176"/>
-      <c r="H83" s="171"/>
-      <c r="I83" s="175"/>
-      <c r="J83" s="173"/>
-      <c r="K83" s="177"/>
-      <c r="L83" s="178" t="str">
+      <c r="H83" s="4"/>
+      <c r="K83" s="81"/>
+      <c r="L83" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="15" customHeight="1">
-      <c r="A84" s="171"/>
-      <c r="B84" s="172"/>
-      <c r="C84" s="173"/>
-      <c r="D84" s="174"/>
-      <c r="E84" s="172" t="str">
+      <c r="A84" s="4"/>
+      <c r="E84" s="1" t="str">
         <f>_xlfn.XLOOKUP(F84,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G84" s="176"/>
-      <c r="H84" s="171"/>
-      <c r="I84" s="175"/>
-      <c r="J84" s="173"/>
-      <c r="K84" s="177"/>
-      <c r="L84" s="178" t="str">
+      <c r="H84" s="4"/>
+      <c r="K84" s="81"/>
+      <c r="L84" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="15" customHeight="1">
-      <c r="A85" s="171"/>
-      <c r="B85" s="172"/>
-      <c r="C85" s="173"/>
-      <c r="D85" s="174"/>
-      <c r="E85" s="172" t="str">
+      <c r="A85" s="4"/>
+      <c r="E85" s="1" t="str">
         <f>_xlfn.XLOOKUP(F85,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G85" s="176"/>
-      <c r="H85" s="171"/>
-      <c r="I85" s="175"/>
-      <c r="J85" s="173"/>
-      <c r="K85" s="177"/>
-      <c r="L85" s="178" t="str">
+      <c r="H85" s="4"/>
+      <c r="K85" s="81"/>
+      <c r="L85" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="15" customHeight="1">
-      <c r="A86" s="171"/>
-      <c r="B86" s="172"/>
-      <c r="C86" s="173"/>
-      <c r="D86" s="174"/>
-      <c r="E86" s="172" t="str">
+      <c r="A86" s="4"/>
+      <c r="E86" s="1" t="str">
         <f>_xlfn.XLOOKUP(F86,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G86" s="176"/>
-      <c r="H86" s="171"/>
-      <c r="I86" s="175"/>
-      <c r="J86" s="173"/>
-      <c r="K86" s="177"/>
-      <c r="L86" s="178" t="str">
+      <c r="H86" s="4"/>
+      <c r="K86" s="81"/>
+      <c r="L86" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="15" customHeight="1">
-      <c r="A87" s="171"/>
-      <c r="B87" s="172"/>
-      <c r="C87" s="173"/>
-      <c r="D87" s="174"/>
-      <c r="E87" s="172" t="str">
+      <c r="A87" s="4"/>
+      <c r="E87" s="1" t="str">
         <f>_xlfn.XLOOKUP(F87,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G87" s="176"/>
-      <c r="H87" s="171"/>
-      <c r="I87" s="175"/>
-      <c r="J87" s="173"/>
-      <c r="K87" s="177"/>
-      <c r="L87" s="178" t="str">
+      <c r="H87" s="4"/>
+      <c r="K87" s="81"/>
+      <c r="L87" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="15" customHeight="1">
-      <c r="A88" s="171"/>
-      <c r="B88" s="172"/>
-      <c r="C88" s="173"/>
-      <c r="D88" s="174"/>
-      <c r="E88" s="172" t="str">
+      <c r="A88" s="4"/>
+      <c r="E88" s="1" t="str">
         <f>_xlfn.XLOOKUP(F88,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G88" s="176"/>
-      <c r="H88" s="171"/>
-      <c r="I88" s="175"/>
-      <c r="J88" s="173"/>
-      <c r="K88" s="177"/>
-      <c r="L88" s="178" t="str">
+      <c r="H88" s="4"/>
+      <c r="K88" s="81"/>
+      <c r="L88" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="15" customHeight="1">
-      <c r="A89" s="171"/>
-      <c r="B89" s="172"/>
-      <c r="C89" s="173"/>
-      <c r="D89" s="174"/>
-      <c r="E89" s="172" t="str">
+      <c r="A89" s="4"/>
+      <c r="E89" s="1" t="str">
         <f>_xlfn.XLOOKUP(F89,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G89" s="176"/>
-      <c r="H89" s="171"/>
-      <c r="I89" s="175"/>
-      <c r="J89" s="173"/>
-      <c r="K89" s="177"/>
-      <c r="L89" s="178" t="str">
+      <c r="H89" s="4"/>
+      <c r="K89" s="81"/>
+      <c r="L89" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="15" customHeight="1">
-      <c r="A90" s="171"/>
-      <c r="B90" s="172"/>
-      <c r="C90" s="173"/>
-      <c r="D90" s="174"/>
-      <c r="E90" s="172" t="str">
+      <c r="A90" s="4"/>
+      <c r="E90" s="1" t="str">
         <f>_xlfn.XLOOKUP(F90,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G90" s="176"/>
-      <c r="H90" s="171"/>
-      <c r="I90" s="175"/>
-      <c r="J90" s="173"/>
-      <c r="K90" s="177"/>
-      <c r="L90" s="178" t="str">
+      <c r="H90" s="4"/>
+      <c r="K90" s="81"/>
+      <c r="L90" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="15" customHeight="1">
-      <c r="A91" s="171"/>
-      <c r="B91" s="172"/>
-      <c r="C91" s="173"/>
-      <c r="D91" s="174"/>
-      <c r="E91" s="172" t="str">
+      <c r="A91" s="4"/>
+      <c r="E91" s="1" t="str">
         <f>_xlfn.XLOOKUP(F91,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G91" s="176"/>
-      <c r="H91" s="171"/>
-      <c r="I91" s="175"/>
-      <c r="J91" s="173"/>
-      <c r="K91" s="177"/>
-      <c r="L91" s="178" t="str">
+      <c r="H91" s="4"/>
+      <c r="K91" s="81"/>
+      <c r="L91" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="15" customHeight="1">
-      <c r="A92" s="171"/>
-      <c r="B92" s="172"/>
-      <c r="C92" s="173"/>
-      <c r="D92" s="174"/>
-      <c r="E92" s="172" t="str">
+      <c r="A92" s="4"/>
+      <c r="E92" s="1" t="str">
         <f>_xlfn.XLOOKUP(F92,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G92" s="176"/>
-      <c r="H92" s="171"/>
-      <c r="I92" s="175"/>
-      <c r="J92" s="173"/>
-      <c r="K92" s="177"/>
-      <c r="L92" s="178" t="str">
+      <c r="H92" s="4"/>
+      <c r="K92" s="81"/>
+      <c r="L92" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="15" customHeight="1">
-      <c r="A93" s="171"/>
-      <c r="B93" s="172"/>
-      <c r="C93" s="173"/>
-      <c r="D93" s="174"/>
-      <c r="E93" s="172" t="str">
+      <c r="A93" s="4"/>
+      <c r="E93" s="1" t="str">
         <f>_xlfn.XLOOKUP(F93,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G93" s="176"/>
-      <c r="H93" s="171"/>
-      <c r="I93" s="175"/>
-      <c r="J93" s="173"/>
-      <c r="K93" s="177"/>
-      <c r="L93" s="178" t="str">
+      <c r="H93" s="4"/>
+      <c r="K93" s="81"/>
+      <c r="L93" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="15" customHeight="1">
-      <c r="A94" s="171"/>
-      <c r="B94" s="172"/>
-      <c r="C94" s="173"/>
-      <c r="D94" s="174"/>
-      <c r="E94" s="172" t="str">
+      <c r="A94" s="4"/>
+      <c r="E94" s="1" t="str">
         <f>_xlfn.XLOOKUP(F94,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G94" s="176"/>
-      <c r="H94" s="171"/>
-      <c r="I94" s="175"/>
-      <c r="J94" s="173"/>
-      <c r="K94" s="177"/>
-      <c r="L94" s="178" t="str">
+      <c r="H94" s="4"/>
+      <c r="K94" s="81"/>
+      <c r="L94" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="15" customHeight="1">
-      <c r="A95" s="171"/>
-      <c r="B95" s="172"/>
-      <c r="C95" s="173"/>
-      <c r="D95" s="174"/>
-      <c r="E95" s="172" t="str">
+      <c r="A95" s="4"/>
+      <c r="E95" s="1" t="str">
         <f>_xlfn.XLOOKUP(F95,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G95" s="176"/>
-      <c r="H95" s="171"/>
-      <c r="I95" s="175"/>
-      <c r="J95" s="173"/>
-      <c r="K95" s="177"/>
-      <c r="L95" s="178" t="str">
+      <c r="H95" s="4"/>
+      <c r="K95" s="81"/>
+      <c r="L95" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="15" customHeight="1">
-      <c r="A96" s="171"/>
-      <c r="B96" s="172"/>
-      <c r="C96" s="173"/>
-      <c r="D96" s="174"/>
-      <c r="E96" s="172" t="str">
+      <c r="A96" s="4"/>
+      <c r="E96" s="1" t="str">
         <f>_xlfn.XLOOKUP(F96,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G96" s="176"/>
-      <c r="H96" s="171"/>
-      <c r="I96" s="175"/>
-      <c r="J96" s="173"/>
-      <c r="K96" s="177"/>
-      <c r="L96" s="178" t="str">
+      <c r="H96" s="4"/>
+      <c r="K96" s="81"/>
+      <c r="L96" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="15" customHeight="1">
-      <c r="A97" s="171"/>
-      <c r="B97" s="172"/>
-      <c r="C97" s="173"/>
-      <c r="D97" s="174"/>
-      <c r="E97" s="172" t="str">
+      <c r="A97" s="4"/>
+      <c r="E97" s="1" t="str">
         <f>_xlfn.XLOOKUP(F97,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G97" s="176"/>
-      <c r="H97" s="171"/>
-      <c r="I97" s="175"/>
-      <c r="J97" s="173"/>
-      <c r="K97" s="177"/>
-      <c r="L97" s="178" t="str">
+      <c r="H97" s="4"/>
+      <c r="K97" s="81"/>
+      <c r="L97" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="15" customHeight="1">
-      <c r="A98" s="171"/>
-      <c r="B98" s="172"/>
-      <c r="C98" s="173"/>
-      <c r="D98" s="174"/>
-      <c r="E98" s="172" t="str">
+      <c r="A98" s="4"/>
+      <c r="E98" s="1" t="str">
         <f>_xlfn.XLOOKUP(F98,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G98" s="176"/>
-      <c r="H98" s="171"/>
-      <c r="I98" s="175"/>
-      <c r="J98" s="173"/>
-      <c r="K98" s="177"/>
-      <c r="L98" s="178" t="str">
+      <c r="H98" s="4"/>
+      <c r="K98" s="81"/>
+      <c r="L98" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="15" customHeight="1">
-      <c r="A99" s="171"/>
-      <c r="B99" s="172"/>
-      <c r="C99" s="173"/>
-      <c r="D99" s="174"/>
-      <c r="E99" s="172" t="str">
+      <c r="A99" s="4"/>
+      <c r="E99" s="1" t="str">
         <f>_xlfn.XLOOKUP(F99,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G99" s="176"/>
-      <c r="H99" s="171"/>
-      <c r="I99" s="175"/>
-      <c r="J99" s="173"/>
-      <c r="K99" s="177"/>
-      <c r="L99" s="178" t="str">
+      <c r="H99" s="4"/>
+      <c r="K99" s="81"/>
+      <c r="L99" s="17" t="str">
         <f t="shared" si="3"/>
         <v>00.01 -Ped  - -R$</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="15" customHeight="1">
-      <c r="A100" s="171"/>
-      <c r="B100" s="172"/>
-      <c r="C100" s="173"/>
-      <c r="D100" s="174"/>
-      <c r="E100" s="172" t="str">
+      <c r="A100" s="4"/>
+      <c r="E100" s="1" t="str">
         <f>_xlfn.XLOOKUP(F100,UTIL!Q:Q,UTIL!N:N,"-")</f>
         <v>0</v>
       </c>
-      <c r="G100" s="176"/>
-      <c r="H100" s="171"/>
-      <c r="I100" s="175"/>
-      <c r="J100" s="173"/>
-      <c r="K100" s="177"/>
-      <c r="L100" s="178" t="str">
+      <c r="H100" s="4"/>
+      <c r="K100" s="81"/>
+      <c r="L100" s="17" t="str">
         <f>TEXT($C100,"dd.mm") &amp; " -Ped " &amp; D100 &amp; " -" &amp; F100 &amp; " -R$" &amp; G100 &amp; IF(LEN(TRIM(I100))=0, "", " -NF " &amp; TRIM(I100))</f>
         <v>00.01 -Ped  - -R$</v>
       </c>
@@ -18965,7 +18756,7 @@
       <c r="K1" s="19" t="s">
         <v>480</v>
       </c>
-      <c r="L1" s="167" t="s">
+      <c r="L1" s="168" t="s">
         <v>329</v>
       </c>
       <c r="N1" s="19" t="s">
@@ -18983,7 +18774,7 @@
       <c r="R1" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="S1" s="167" t="s">
+      <c r="S1" s="168" t="s">
         <v>485</v>
       </c>
       <c r="U1" s="7">
@@ -19038,7 +18829,7 @@
         <f>"A:"&amp;TEXT(F2,"0,00")&amp;" x C:"&amp;TEXT(G2,"0,00")&amp;" x L:"&amp;TEXT(H2,"0,00")&amp;"-"&amp;TEXT(I2,"0,00")&amp;" x P:"&amp;TEXT(J2,"0.00")&amp;"kg"</f>
         <v>A:2,28 x C:3,10 x L:1,00-1,57 x P:1.200kg</v>
       </c>
-      <c r="L2" s="167"/>
+      <c r="L2" s="168"/>
       <c r="N2" s="20" t="str">
         <f t="shared" ref="N2:N65" si="0">"0"&amp;LEFT(TEXT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(O2,".",""),"/",""),"-",""),"00000000000000"),8)</f>
         <v>020920599</v>
@@ -19055,7 +18846,7 @@
       <c r="R2" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="S2" s="167"/>
+      <c r="S2" s="168"/>
       <c r="V2" s="8" t="s">
         <v>495</v>
       </c>
@@ -19102,7 +18893,7 @@
         <f t="shared" ref="K3:K66" si="1">"A:"&amp;TEXT(F3,"0,00")&amp;" x C:"&amp;TEXT(G3,"0,00")&amp;" x L:"&amp;TEXT(H3,"0,00")&amp;"-"&amp;TEXT(I3,"0,00")&amp;" x P:"&amp;TEXT(J3,"0.00")&amp;"kg"</f>
         <v>A:2,60 x C:4,08 x L:1,45-2,00 x P:5.100kg</v>
       </c>
-      <c r="L3" s="167"/>
+      <c r="L3" s="168"/>
       <c r="N3" s="20" t="str">
         <f t="shared" si="0"/>
         <v>019320206</v>
@@ -19119,7 +18910,7 @@
       <c r="R3" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="S3" s="167"/>
+      <c r="S3" s="168"/>
       <c r="U3" s="7">
         <v>2</v>
       </c>
@@ -19172,7 +18963,7 @@
         <f t="shared" si="1"/>
         <v>A:2,38 x C:4,08 x L:1,44-1,88 x P:2.710kg</v>
       </c>
-      <c r="L4" s="167"/>
+      <c r="L4" s="168"/>
       <c r="N4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>044160580</v>
@@ -19189,7 +18980,7 @@
       <c r="R4" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="S4" s="167"/>
+      <c r="S4" s="168"/>
       <c r="V4" s="8" t="s">
         <v>510</v>
       </c>
@@ -19236,7 +19027,7 @@
         <f t="shared" si="1"/>
         <v>A:2,38 x C:4,08 x L:1,44-1,88 x P:2.710kg</v>
       </c>
-      <c r="L5" s="167"/>
+      <c r="L5" s="168"/>
       <c r="N5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>048501079</v>
@@ -19253,7 +19044,7 @@
       <c r="R5" s="20" t="s">
         <v>516</v>
       </c>
-      <c r="S5" s="167"/>
+      <c r="S5" s="168"/>
       <c r="U5" s="7">
         <v>3</v>
       </c>
@@ -19306,7 +19097,7 @@
         <f t="shared" si="1"/>
         <v>A:2,60 x C:4,08 x L:1,45-2,00 x P:5.100kg</v>
       </c>
-      <c r="L6" s="167"/>
+      <c r="L6" s="168"/>
       <c r="N6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>031553361</v>
@@ -19323,7 +19114,7 @@
       <c r="R6" s="20" t="s">
         <v>525</v>
       </c>
-      <c r="S6" s="167"/>
+      <c r="S6" s="168"/>
       <c r="V6" s="8" t="s">
         <v>526</v>
       </c>
@@ -19372,7 +19163,7 @@
         <f t="shared" si="1"/>
         <v>A:2,77 x C:4,17 x L:1,45-2,00 x P:5.100kg</v>
       </c>
-      <c r="L7" s="167"/>
+      <c r="L7" s="168"/>
       <c r="N7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>050435638</v>
@@ -19389,7 +19180,7 @@
       <c r="R7" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="S7" s="167"/>
+      <c r="S7" s="168"/>
       <c r="U7" s="7">
         <v>4</v>
       </c>
@@ -19442,7 +19233,7 @@
         <f t="shared" si="1"/>
         <v>A:2,60 x C:4,08 x L:1,45-2,00 x P:5.100kg</v>
       </c>
-      <c r="L8" s="167"/>
+      <c r="L8" s="168"/>
       <c r="N8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>046570181</v>
@@ -19459,7 +19250,7 @@
       <c r="R8" s="20" t="s">
         <v>525</v>
       </c>
-      <c r="S8" s="167"/>
+      <c r="S8" s="168"/>
       <c r="V8" s="8" t="s">
         <v>541</v>
       </c>
@@ -19506,7 +19297,7 @@
         <f t="shared" si="1"/>
         <v>A:2,77 x C:4,17 x L:1,45-2,00 x P:5.100kg</v>
       </c>
-      <c r="L9" s="167"/>
+      <c r="L9" s="168"/>
       <c r="N9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>061196032</v>
@@ -19523,7 +19314,7 @@
       <c r="R9" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="S9" s="167"/>
+      <c r="S9" s="168"/>
       <c r="U9" s="7">
         <v>5</v>
       </c>
@@ -19576,7 +19367,7 @@
         <f t="shared" si="1"/>
         <v>A:2,72 x C:4,56 x L:2,50-3,30 x P:5.600kg</v>
       </c>
-      <c r="L10" s="167"/>
+      <c r="L10" s="168"/>
       <c r="N10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>030712609</v>
@@ -19593,7 +19384,7 @@
       <c r="R10" s="20" t="s">
         <v>516</v>
       </c>
-      <c r="S10" s="167"/>
+      <c r="S10" s="168"/>
       <c r="V10" s="8" t="s">
         <v>555</v>
       </c>
@@ -19640,7 +19431,7 @@
         <f t="shared" si="1"/>
         <v>A:2,72 x C:4,56 x L:2,60-3,30 x P:6.300kg</v>
       </c>
-      <c r="L11" s="167"/>
+      <c r="L11" s="168"/>
       <c r="N11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>018492099</v>
@@ -19657,7 +19448,7 @@
       <c r="R11" s="20" t="s">
         <v>561</v>
       </c>
-      <c r="S11" s="167"/>
+      <c r="S11" s="168"/>
       <c r="U11" s="7">
         <v>6</v>
       </c>
@@ -19710,7 +19501,7 @@
         <f t="shared" si="1"/>
         <v>A:2,72 x C:4,56 x L:2,70-3,35 x P:6.800kg</v>
       </c>
-      <c r="L12" s="167"/>
+      <c r="L12" s="168"/>
       <c r="N12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>038052835</v>
@@ -19727,7 +19518,7 @@
       <c r="R12" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="S12" s="167"/>
+      <c r="S12" s="168"/>
       <c r="V12" s="8" t="s">
         <v>569</v>
       </c>
@@ -19774,7 +19565,7 @@
         <f t="shared" si="1"/>
         <v>A:2,74 x C:4,92 x L:2,87-3,45 x P:7.200kg</v>
       </c>
-      <c r="L13" s="167"/>
+      <c r="L13" s="168"/>
       <c r="N13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>055246903</v>
@@ -19791,7 +19582,7 @@
       <c r="R13" s="20" t="s">
         <v>575</v>
       </c>
-      <c r="S13" s="167"/>
+      <c r="S13" s="168"/>
       <c r="U13" s="7">
         <v>7</v>
       </c>
@@ -19844,7 +19635,7 @@
         <f t="shared" si="1"/>
         <v>A:2,28 x C:4,56 x L:2,87-3,45 x P:7.500kg</v>
       </c>
-      <c r="L14" s="167"/>
+      <c r="L14" s="168"/>
       <c r="N14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>006208105</v>
@@ -19861,7 +19652,7 @@
       <c r="R14" s="20" t="s">
         <v>582</v>
       </c>
-      <c r="S14" s="167"/>
+      <c r="S14" s="168"/>
       <c r="V14" s="8" t="s">
         <v>583</v>
       </c>
@@ -19908,7 +19699,7 @@
         <f t="shared" si="1"/>
         <v>A:2,86 x C:4,96 x L:2,70-3,30 x P:7.800kg</v>
       </c>
-      <c r="L15" s="167"/>
+      <c r="L15" s="168"/>
       <c r="N15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>006208105</v>
@@ -19925,7 +19716,7 @@
       <c r="R15" s="20" t="s">
         <v>588</v>
       </c>
-      <c r="S15" s="167"/>
+      <c r="S15" s="168"/>
       <c r="U15" s="7">
         <v>8</v>
       </c>
@@ -19978,7 +19769,7 @@
         <f t="shared" si="1"/>
         <v>A:2,93 x C:4,65 x L:2,70-3,30 x P:8.500kg</v>
       </c>
-      <c r="L16" s="167"/>
+      <c r="L16" s="168"/>
       <c r="N16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>006208105</v>
@@ -19995,7 +19786,7 @@
       <c r="R16" s="20" t="s">
         <v>594</v>
       </c>
-      <c r="S16" s="167"/>
+      <c r="S16" s="168"/>
       <c r="V16" s="8" t="s">
         <v>595</v>
       </c>
@@ -20042,7 +19833,7 @@
         <f t="shared" si="1"/>
         <v>A:2,93 x C:5,42 x L:2,74-3,40 x P:8.500kg</v>
       </c>
-      <c r="L17" s="167"/>
+      <c r="L17" s="168"/>
       <c r="N17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>006208105</v>
@@ -20059,7 +19850,7 @@
       <c r="R17" s="20" t="s">
         <v>600</v>
       </c>
-      <c r="S17" s="167"/>
+      <c r="S17" s="168"/>
       <c r="V17" s="7"/>
       <c r="W17" s="54" t="s">
         <v>601</v>
@@ -20107,7 +19898,7 @@
         <f t="shared" si="1"/>
         <v>A:3,30 x C:5,24 x L:2,74-3,40 x P:9.550kg</v>
       </c>
-      <c r="L18" s="167"/>
+      <c r="L18" s="168"/>
       <c r="N18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>006208105</v>
@@ -20124,7 +19915,7 @@
       <c r="R18" s="20" t="s">
         <v>606</v>
       </c>
-      <c r="S18" s="167"/>
+      <c r="S18" s="168"/>
       <c r="V18" s="7"/>
       <c r="W18" s="54" t="s">
         <v>607</v>
@@ -20174,7 +19965,7 @@
         <f t="shared" si="1"/>
         <v>A:2,98 x C:5,42 x L:2,95-3,60 x P:9.800kg</v>
       </c>
-      <c r="L19" s="167"/>
+      <c r="L19" s="168"/>
       <c r="N19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>006208105</v>
@@ -20191,7 +19982,7 @@
       <c r="R19" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="S19" s="167"/>
+      <c r="S19" s="168"/>
       <c r="V19" s="7"/>
       <c r="Y19" s="56" t="s">
         <v>615</v>
@@ -20238,7 +20029,7 @@
         <f t="shared" si="1"/>
         <v>A:3,30 x C:5,24 x L:2,95-3,60 x P:10.650kg</v>
       </c>
-      <c r="L20" s="167"/>
+      <c r="L20" s="168"/>
       <c r="N20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>006208105</v>
@@ -20255,7 +20046,7 @@
       <c r="R20" s="20" t="s">
         <v>619</v>
       </c>
-      <c r="S20" s="167"/>
+      <c r="S20" s="168"/>
       <c r="V20" s="19" t="s">
         <v>620</v>
       </c>
@@ -20622,11 +20413,11 @@
         <v>657</v>
       </c>
       <c r="W26" s="7"/>
-      <c r="Y26" s="168" t="s">
+      <c r="Y26" s="169" t="s">
         <v>658</v>
       </c>
-      <c r="Z26" s="168"/>
-      <c r="AA26" s="168"/>
+      <c r="Z26" s="169"/>
+      <c r="AA26" s="169"/>
     </row>
     <row r="27" spans="1:27">
       <c r="A27" s="20">
@@ -28061,10 +27852,10 @@
       <c r="G13" s="111"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="K15" s="170" t="s">
+      <c r="K15" s="171" t="s">
         <v>1215</v>
       </c>
-      <c r="L15" s="170"/>
+      <c r="L15" s="171"/>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" s="130" t="s">
@@ -28365,7 +28156,7 @@
     </row>
     <row r="33" spans="2:12">
       <c r="B33" s="90"/>
-      <c r="K33" s="169" t="s">
+      <c r="K33" s="170" t="s">
         <v>1234</v>
       </c>
       <c r="L33" s="139" t="s">
@@ -28373,7 +28164,7 @@
       </c>
     </row>
     <row r="34" spans="2:12" ht="14.45">
-      <c r="K34" s="169"/>
+      <c r="K34" s="170"/>
       <c r="L34" s="137" t="s">
         <v>248</v>
       </c>
@@ -28407,10 +28198,10 @@
       <c r="L38" s="142"/>
     </row>
     <row r="39" spans="2:12">
-      <c r="K39" s="170" t="s">
+      <c r="K39" s="171" t="s">
         <v>1240</v>
       </c>
-      <c r="L39" s="170"/>
+      <c r="L39" s="171"/>
     </row>
     <row r="40" spans="2:12">
       <c r="K40" s="139" t="s">
@@ -28477,7 +28268,7 @@
       </c>
     </row>
     <row r="49" spans="11:12">
-      <c r="K49" s="169" t="s">
+      <c r="K49" s="170" t="s">
         <v>1234</v>
       </c>
       <c r="L49" s="139" t="s">
@@ -28485,7 +28276,7 @@
       </c>
     </row>
     <row r="50" spans="11:12" ht="14.45">
-      <c r="K50" s="169"/>
+      <c r="K50" s="170"/>
       <c r="L50" s="137" t="s">
         <v>278</v>
       </c>
@@ -28519,10 +28310,10 @@
       <c r="L54" s="142"/>
     </row>
     <row r="55" spans="11:12">
-      <c r="K55" s="170" t="s">
+      <c r="K55" s="171" t="s">
         <v>1244</v>
       </c>
-      <c r="L55" s="170"/>
+      <c r="L55" s="171"/>
     </row>
     <row r="56" spans="11:12">
       <c r="K56" s="139" t="s">
@@ -28588,7 +28379,7 @@
       </c>
     </row>
     <row r="65" spans="11:12">
-      <c r="K65" s="169" t="s">
+      <c r="K65" s="170" t="s">
         <v>1234</v>
       </c>
       <c r="L65" s="139" t="s">
@@ -28596,7 +28387,7 @@
       </c>
     </row>
     <row r="66" spans="11:12" ht="14.45">
-      <c r="K66" s="169"/>
+      <c r="K66" s="170"/>
       <c r="L66" s="137" t="s">
         <v>286</v>
       </c>
@@ -28630,10 +28421,10 @@
       <c r="L70" s="142"/>
     </row>
     <row r="71" spans="11:12">
-      <c r="K71" s="170" t="s">
+      <c r="K71" s="171" t="s">
         <v>1248</v>
       </c>
-      <c r="L71" s="170"/>
+      <c r="L71" s="171"/>
     </row>
     <row r="72" spans="11:12">
       <c r="K72" s="139" t="s">
@@ -28700,7 +28491,7 @@
       </c>
     </row>
     <row r="81" spans="2:12">
-      <c r="K81" s="169" t="s">
+      <c r="K81" s="170" t="s">
         <v>1234</v>
       </c>
       <c r="L81" s="139" t="s">
@@ -28708,7 +28499,7 @@
       </c>
     </row>
     <row r="82" spans="2:12" ht="14.45">
-      <c r="K82" s="169"/>
+      <c r="K82" s="170"/>
       <c r="L82" s="146" t="s">
         <v>294</v>
       </c>
@@ -28742,10 +28533,10 @@
       <c r="L86" s="142"/>
     </row>
     <row r="87" spans="2:12">
-      <c r="K87" s="170" t="s">
+      <c r="K87" s="171" t="s">
         <v>1251</v>
       </c>
-      <c r="L87" s="170"/>
+      <c r="L87" s="171"/>
     </row>
     <row r="88" spans="2:12">
       <c r="K88" s="139" t="s">
@@ -28874,7 +28665,7 @@
       </c>
     </row>
     <row r="101" spans="6:12">
-      <c r="K101" s="169" t="s">
+      <c r="K101" s="170" t="s">
         <v>1234</v>
       </c>
       <c r="L101" s="139" t="s">
@@ -28882,7 +28673,7 @@
       </c>
     </row>
     <row r="102" spans="6:12" ht="20.25" customHeight="1">
-      <c r="K102" s="169"/>
+      <c r="K102" s="170"/>
       <c r="L102" s="146" t="s">
         <v>297</v>
       </c>
@@ -28918,10 +28709,10 @@
     <row r="107" spans="6:12">
       <c r="F107" s="123"/>
       <c r="G107" s="125"/>
-      <c r="K107" s="170" t="s">
+      <c r="K107" s="171" t="s">
         <v>1254</v>
       </c>
-      <c r="L107" s="170"/>
+      <c r="L107" s="171"/>
     </row>
     <row r="108" spans="6:12">
       <c r="F108" s="122"/>
@@ -29030,7 +28821,7 @@
       </c>
     </row>
     <row r="125" spans="11:12" ht="14.45">
-      <c r="K125" s="169" t="s">
+      <c r="K125" s="170" t="s">
         <v>1234</v>
       </c>
       <c r="L125" s="136" t="s">
@@ -29038,7 +28829,7 @@
       </c>
     </row>
     <row r="126" spans="11:12" ht="14.45">
-      <c r="K126" s="169"/>
+      <c r="K126" s="170"/>
       <c r="L126" s="146" t="s">
         <v>1256</v>
       </c>
@@ -29072,10 +28863,10 @@
       <c r="L130" s="142"/>
     </row>
     <row r="131" spans="11:12">
-      <c r="K131" s="170" t="s">
+      <c r="K131" s="171" t="s">
         <v>1257</v>
       </c>
-      <c r="L131" s="170"/>
+      <c r="L131" s="171"/>
     </row>
     <row r="132" spans="11:12">
       <c r="K132" s="139" t="s">
@@ -29182,7 +28973,7 @@
       </c>
     </row>
     <row r="149" spans="11:12" ht="14.45">
-      <c r="K149" s="169" t="s">
+      <c r="K149" s="170" t="s">
         <v>1234</v>
       </c>
       <c r="L149" s="136" t="s">
@@ -29190,7 +28981,7 @@
       </c>
     </row>
     <row r="150" spans="11:12" ht="14.45">
-      <c r="K150" s="169"/>
+      <c r="K150" s="170"/>
       <c r="L150" s="137" t="s">
         <v>305</v>
       </c>
@@ -29406,28 +29197,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="97552bd7-0050-4a40-a3e9-7eed99743892" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f9af305-95c5-4ec5-a7fe-f235b5fb43bb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100165C9838A8BE0240B14ECB57A7D15C1B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="b1e3a46b5aabf9910121de6df837e2f4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f9af305-95c5-4ec5-a7fe-f235b5fb43bb" xmlns:ns3="97552bd7-0050-4a40-a3e9-7eed99743892" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a8bcdd80e11db0abec65d927b8f8cf5e" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100165C9838A8BE0240B14ECB57A7D15C1B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="38153ec566ff0f4bf479b7a6c9088949">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f9af305-95c5-4ec5-a7fe-f235b5fb43bb" xmlns:ns3="97552bd7-0050-4a40-a3e9-7eed99743892" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05d834da23fbd08f588ccb0f92beec26" ns2:_="" ns3:_="">
     <xsd:import namespace="1f9af305-95c5-4ec5-a7fe-f235b5fb43bb"/>
     <xsd:import namespace="97552bd7-0050-4a40-a3e9-7eed99743892"/>
     <xsd:element name="properties">
@@ -29620,8 +29391,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="97552bd7-0050-4a40-a3e9-7eed99743892" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1f9af305-95c5-4ec5-a7fe-f235b5fb43bb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245723BA-9722-4970-B575-35956A766521}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F68AB9D-41AE-4D08-9FF6-738980CEC4EB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29629,5 +29420,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4045654C-FB36-49BB-9133-FC21DAF655AA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245723BA-9722-4970-B575-35956A766521}"/>
 </file>
</xml_diff>